<commit_message>
lexico implementado em Tabela de .
ainda falta implementar a tabela de caracteres especiais e tabela de
Palavras reservadas.
</commit_message>
<xml_diff>
--- a/Documentos/tabela de tokens.xlsx
+++ b/Documentos/tabela de tokens.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="76">
   <si>
     <t>Terminal</t>
   </si>
@@ -274,12 +274,24 @@
   <si>
     <t>FLOAT</t>
   </si>
+  <si>
+    <t>(\[)</t>
+  </si>
+  <si>
+    <t>(\])</t>
+  </si>
+  <si>
+    <t>RIGHTCOLCH</t>
+  </si>
+  <si>
+    <t>LEFTCOLCH</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -313,6 +325,12 @@
       <sz val="15"/>
       <color theme="1"/>
       <name val="Cambria"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -390,8 +408,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -451,19 +471,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -793,17 +815,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.33203125" customWidth="1"/>
-    <col min="3" max="3" width="21.83203125" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1096,7 +1118,7 @@
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="12"/>
+      <c r="A24" s="11"/>
       <c r="B24" s="2" t="s">
         <v>58</v>
       </c>
@@ -1107,128 +1129,154 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="16">
-      <c r="A25" s="2" t="s">
+    <row r="25" spans="1:4">
+      <c r="A25" s="11"/>
+      <c r="B25" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="12"/>
+      <c r="B26" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="16">
+      <c r="A27" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B27" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="20">
-      <c r="A26" s="2" t="s">
+    <row r="28" spans="1:4" ht="20">
+      <c r="A28" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B28" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="30" customHeight="1">
-      <c r="B28" s="13" t="s">
+    <row r="30" spans="1:4" ht="30" customHeight="1">
+      <c r="B30" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="C28" s="13"/>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="B29" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C29" s="6">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="B30" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30" s="6">
-        <v>257</v>
-      </c>
+      <c r="C30" s="13"/>
     </row>
     <row r="31" spans="1:4">
       <c r="B31" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C31" s="6">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="B32" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C32" s="6">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="33" spans="2:3">
       <c r="B33" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C33" s="6">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="34" spans="2:3">
       <c r="B34" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C34" s="6">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="35" spans="2:3">
       <c r="B35" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C35" s="6">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="36" spans="2:3">
       <c r="B36" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" s="6">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3">
+      <c r="B37" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C37" s="6">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3">
+      <c r="B38" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C36" s="6">
+      <c r="C38" s="6">
         <v>263</v>
       </c>
     </row>
-    <row r="37" spans="2:3">
-      <c r="B37" s="9" t="s">
+    <row r="39" spans="2:3">
+      <c r="B39" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C37" s="6">
+      <c r="C39" s="6">
         <v>264</v>
       </c>
     </row>
-    <row r="38" spans="2:3">
-      <c r="B38" s="9" t="s">
+    <row r="40" spans="2:3">
+      <c r="B40" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C38" s="6">
+      <c r="C40" s="6">
         <v>265</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A8:A24"/>
-    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="A8:A26"/>
+    <mergeCell ref="B30:C30"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A2:A3"/>
   </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="4294967294"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>